<commit_message>
HLR excel sheet for saucedemo.com
HLR excel sheet for saucedemo.com inside all 4 user
</commit_message>
<xml_diff>
--- a/Assignment/HLR excel sheet/hlr for loked out user.xlsx
+++ b/Assignment/HLR excel sheet/hlr for loked out user.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ATRI ENTERPRISE\Documents\GitHub\Nirav_Tops\Assignment\HLR excel sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A618E80-4479-4E94-B280-848118BE0317}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{323CED8C-3C08-4F0D-ABF1-0E321EB843C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -482,7 +482,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>